<commit_message>
work with multilple rows, update checkboxes, test
</commit_message>
<xml_diff>
--- a/K-1 Import.xlsx
+++ b/K-1 Import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\az_dev\UPWORK\excel-to-pdf-form.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BF3240-FA22-4F50-8A78-7C84EA0D7A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F072E56B-700F-49B0-AD66-42CFA534A471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9E99ED55-509C-4BCA-89A4-BA783496F3A8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>partner_id</t>
   </si>
@@ -76,12 +76,6 @@
   </si>
   <si>
     <t>New York</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Square Garden</t>
@@ -460,7 +454,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,14 +538,14 @@
       <c r="I2">
         <v>3000</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -562,10 +556,10 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>1234</v>
@@ -579,14 +573,14 @@
       <c r="I3">
         <v>4000</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -597,13 +591,13 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
       </c>
       <c r="F4">
         <v>5321</v>
@@ -617,14 +611,14 @@
       <c r="I4">
         <v>5000</v>
       </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pdf and excel files
</commit_message>
<xml_diff>
--- a/K-1 Import.xlsx
+++ b/K-1 Import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\az_dev\UPWORK\excel-to-pdf-form.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F072E56B-700F-49B0-AD66-42CFA534A471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E03C7F-DE0D-40C9-A7D2-3DCCF387BA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9E99ED55-509C-4BCA-89A4-BA783496F3A8}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,13 +612,13 @@
         <v>5000</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
       </c>
       <c r="L4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>